<commit_message>
Translation based on excel file.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -7,16 +7,14 @@
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Localization" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t>Default</t>
   </si>
@@ -172,14 +170,31 @@
   </si>
   <si>
     <t>Ambos</t>
+  </si>
+  <si>
+    <t>GameMenus.MissionSelection</t>
+  </si>
+  <si>
+    <t>Mission Selection</t>
+  </si>
+  <si>
+    <t>Seleção de Missão</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -207,9 +222,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,32 +749,25 @@
         <v>36</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Mission selection with mission data.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Postgrad\Projeto Final\Project\quest-for-the-crown-3d\Game\Assets\Localization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="129">
   <si>
     <t>Default</t>
   </si>
@@ -194,6 +199,213 @@
   </si>
   <si>
     <t>Aprenda como ser um caçador de tesouros.</t>
+  </si>
+  <si>
+    <t>UI.Prizes</t>
+  </si>
+  <si>
+    <t>Recompensas:</t>
+  </si>
+  <si>
+    <t>Prizes:</t>
+  </si>
+  <si>
+    <t>Common.Money</t>
+  </si>
+  <si>
+    <t>Common.HealthPotion</t>
+  </si>
+  <si>
+    <t>Common.MagicPotion</t>
+  </si>
+  <si>
+    <t>Common.Bomb</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Ouro</t>
+  </si>
+  <si>
+    <t>Health Potion</t>
+  </si>
+  <si>
+    <t>Poção de Vida</t>
+  </si>
+  <si>
+    <t>Magic Potion</t>
+  </si>
+  <si>
+    <t>Poção de Magia</t>
+  </si>
+  <si>
+    <t>Bomb</t>
+  </si>
+  <si>
+    <t>Bomba</t>
+  </si>
+  <si>
+    <t>Mission.Title01</t>
+  </si>
+  <si>
+    <t>Mission.Description01</t>
+  </si>
+  <si>
+    <t>Mission.Title02</t>
+  </si>
+  <si>
+    <t>Mission.Description02</t>
+  </si>
+  <si>
+    <t>Mission.Title03</t>
+  </si>
+  <si>
+    <t>Mission.Description03</t>
+  </si>
+  <si>
+    <t>Mission.Title04</t>
+  </si>
+  <si>
+    <t>Mission.Description04</t>
+  </si>
+  <si>
+    <t>Mission.Title05</t>
+  </si>
+  <si>
+    <t>Mission.Description05</t>
+  </si>
+  <si>
+    <t>Mission.Title06</t>
+  </si>
+  <si>
+    <t>Mission.Description06</t>
+  </si>
+  <si>
+    <t>Mission.Title07</t>
+  </si>
+  <si>
+    <t>Mission.Description07</t>
+  </si>
+  <si>
+    <t>Mission.Title08</t>
+  </si>
+  <si>
+    <t>Mission.Description08</t>
+  </si>
+  <si>
+    <t>Mission.Title09</t>
+  </si>
+  <si>
+    <t>Mission.Description09</t>
+  </si>
+  <si>
+    <t>Kill Some Worms</t>
+  </si>
+  <si>
+    <t>Worms Attacked the Forest. Kill them.</t>
+  </si>
+  <si>
+    <t>Get your bow!</t>
+  </si>
+  <si>
+    <t>Get your bow and kill a few long ranged enemies.</t>
+  </si>
+  <si>
+    <t>Bow Practice</t>
+  </si>
+  <si>
+    <t>Kill enemies and solve puzzles with the bow.</t>
+  </si>
+  <si>
+    <t>Get the fireball spell on the catacombs.</t>
+  </si>
+  <si>
+    <t>Do some magic!</t>
+  </si>
+  <si>
+    <t>Haunted Boomerang.</t>
+  </si>
+  <si>
+    <t>Explore a dark dungeon and kill some enemies with your magic.</t>
+  </si>
+  <si>
+    <t>People say the dark forest guards a treasure. Investigate it!</t>
+  </si>
+  <si>
+    <t>Boomerang practice</t>
+  </si>
+  <si>
+    <t>Kill waves after waves of enemies with the help of your boomerang!</t>
+  </si>
+  <si>
+    <t>The Royal Crypts</t>
+  </si>
+  <si>
+    <t>Find the secret of the abandoned royal crypts.</t>
+  </si>
+  <si>
+    <t>Get the crown!</t>
+  </si>
+  <si>
+    <t>Kill the monsters and recover the crown!</t>
+  </si>
+  <si>
+    <t>Mate algumas Minhocas</t>
+  </si>
+  <si>
+    <t>Minhocas atacaram a floresta. Mate-as.</t>
+  </si>
+  <si>
+    <t>Obtenha seu arco!</t>
+  </si>
+  <si>
+    <t>Obtenha seu arco e mate alguns inimigos com ataques de longo alcance.</t>
+  </si>
+  <si>
+    <t>Prática de Arco e Flecha</t>
+  </si>
+  <si>
+    <t>Mate inimigos e resolva quebra-cabeças com seu arco.</t>
+  </si>
+  <si>
+    <t>Aprenda magia!</t>
+  </si>
+  <si>
+    <t>Learn some Magic!</t>
+  </si>
+  <si>
+    <t>Obtenha a magia da bola de fogo nas catacombas.</t>
+  </si>
+  <si>
+    <t>Pratique magia!</t>
+  </si>
+  <si>
+    <t>Explore um calabouço escuro e mate alguns inimigos com sua magia.</t>
+  </si>
+  <si>
+    <t>Bumerangue mal-assombrado.</t>
+  </si>
+  <si>
+    <t>Rumores dizem que a floresta negra guarda um grande tesouro. Investigue!</t>
+  </si>
+  <si>
+    <t>Prática de Bumerangue</t>
+  </si>
+  <si>
+    <t>Mate hordas de inimigos com a ajuda do seu bumerangue!</t>
+  </si>
+  <si>
+    <t>Criptas Reais</t>
+  </si>
+  <si>
+    <t>Ache o segredo das criptas reais abandonadas.</t>
+  </si>
+  <si>
+    <t>Recupere a coroa!</t>
+  </si>
+  <si>
+    <t>Mate os monstros e recupere a coroa!</t>
   </si>
 </sst>
 </file>
@@ -251,6 +463,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -298,7 +513,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -333,7 +548,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -542,17 +757,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="48.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -798,8 +1013,258 @@
       </c>
       <c r="D22" s="2"/>
     </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
+      <c r="A25" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Option Selection on Camp Screen.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="141">
   <si>
     <t>Default</t>
   </si>
@@ -406,6 +406,42 @@
   </si>
   <si>
     <t>Mate os monstros e recupere a coroa!</t>
+  </si>
+  <si>
+    <t>Dialog.WhatToDo</t>
+  </si>
+  <si>
+    <t>What to do now?</t>
+  </si>
+  <si>
+    <t>O que farei agora?</t>
+  </si>
+  <si>
+    <t>Dialog.GoToMission</t>
+  </si>
+  <si>
+    <t>Do a Mission</t>
+  </si>
+  <si>
+    <t>Fazer uma Missão</t>
+  </si>
+  <si>
+    <t>Dialog.Shop</t>
+  </si>
+  <si>
+    <t>Shop</t>
+  </si>
+  <si>
+    <t>Comprar Suprimentos</t>
+  </si>
+  <si>
+    <t>Ficar no Acampamento</t>
+  </si>
+  <si>
+    <t>Stay at Camp</t>
+  </si>
+  <si>
+    <t>Dialog.StayCamp</t>
   </si>
 </sst>
 </file>
@@ -757,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,6 +1302,53 @@
         <v>128</v>
       </c>
     </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>129</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>135</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>140</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Mission 02 complete. Weapon Chest done.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="165">
   <si>
     <t>Default</t>
   </si>
@@ -487,6 +487,33 @@
   </si>
   <si>
     <t>Voltar à Tela de Titulo</t>
+  </si>
+  <si>
+    <t>Objective.GetBow</t>
+  </si>
+  <si>
+    <t>Get Magic Bow</t>
+  </si>
+  <si>
+    <t>Obter Arco Mágico</t>
+  </si>
+  <si>
+    <t>Mission.Complete01</t>
+  </si>
+  <si>
+    <t>Mission.Complete02</t>
+  </si>
+  <si>
+    <t>You killed 15 worms!</t>
+  </si>
+  <si>
+    <t>Você matou 15 Minhocas!</t>
+  </si>
+  <si>
+    <t>You got your bow!</t>
+  </si>
+  <si>
+    <t>Você obteve o arco!</t>
   </si>
 </sst>
 </file>
@@ -838,10 +865,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,8 +1473,38 @@
         <v>155</v>
       </c>
     </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
WIP: Mission 03 Map.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -868,7 +868,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,7 +1499,7 @@
       <c r="A57" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>163</v>
       </c>
       <c r="C57" s="1" t="s">

</xml_diff>

<commit_message>
Revamped mission count and objectives.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="189">
   <si>
     <t>Default</t>
   </si>
@@ -276,30 +276,6 @@
     <t>Mission.Description05</t>
   </si>
   <si>
-    <t>Mission.Title06</t>
-  </si>
-  <si>
-    <t>Mission.Description06</t>
-  </si>
-  <si>
-    <t>Mission.Title07</t>
-  </si>
-  <si>
-    <t>Mission.Description07</t>
-  </si>
-  <si>
-    <t>Mission.Title08</t>
-  </si>
-  <si>
-    <t>Mission.Description08</t>
-  </si>
-  <si>
-    <t>Mission.Title09</t>
-  </si>
-  <si>
-    <t>Mission.Description09</t>
-  </si>
-  <si>
     <t>Kill Some Worms</t>
   </si>
   <si>
@@ -315,9 +291,6 @@
     <t>Bow Practice</t>
   </si>
   <si>
-    <t>Kill enemies and solve puzzles with the bow.</t>
-  </si>
-  <si>
     <t>Get the fireball spell on the catacombs.</t>
   </si>
   <si>
@@ -366,9 +339,6 @@
     <t>Prática de Arco e Flecha</t>
   </si>
   <si>
-    <t>Mate inimigos e resolva quebra-cabeças com seu arco.</t>
-  </si>
-  <si>
     <t>Aprenda magia!</t>
   </si>
   <si>
@@ -514,6 +484,108 @@
   </si>
   <si>
     <t>Você obteve o arco!</t>
+  </si>
+  <si>
+    <t>Kill long-ranged enemies with the bow.</t>
+  </si>
+  <si>
+    <t>Mate inimigos distantes com seu arco.</t>
+  </si>
+  <si>
+    <t>Mission.Complete03</t>
+  </si>
+  <si>
+    <t>Mission.Complete04</t>
+  </si>
+  <si>
+    <t>Mission.Complete05</t>
+  </si>
+  <si>
+    <t>OldMission.Title03</t>
+  </si>
+  <si>
+    <t>OldMission.Description03</t>
+  </si>
+  <si>
+    <t>OldMission.Title04</t>
+  </si>
+  <si>
+    <t>OldMission.Description04</t>
+  </si>
+  <si>
+    <t>OldMission.Title05</t>
+  </si>
+  <si>
+    <t>OldMission.Description05</t>
+  </si>
+  <si>
+    <t>OldMission.Title06</t>
+  </si>
+  <si>
+    <t>OldMission.Description06</t>
+  </si>
+  <si>
+    <t>OldMission.Title07</t>
+  </si>
+  <si>
+    <t>OldMission.Description07</t>
+  </si>
+  <si>
+    <t>OldMission.Title08</t>
+  </si>
+  <si>
+    <t>OldMission.Description08</t>
+  </si>
+  <si>
+    <t>OldMission.Title09</t>
+  </si>
+  <si>
+    <t>OldMission.Description09</t>
+  </si>
+  <si>
+    <t>Objective.KillMagyplus</t>
+  </si>
+  <si>
+    <t>Kill Magyplus</t>
+  </si>
+  <si>
+    <t>Mate Magotorrincos</t>
+  </si>
+  <si>
+    <t>Objective.GetFireball</t>
+  </si>
+  <si>
+    <t>Obtain Fireball magic</t>
+  </si>
+  <si>
+    <t>Obtenha a magia Bola de Fogo</t>
+  </si>
+  <si>
+    <t>Objective.GetBoomerang</t>
+  </si>
+  <si>
+    <t>Obtain Boomerang</t>
+  </si>
+  <si>
+    <t>Obtenha o bumerangue</t>
+  </si>
+  <si>
+    <t>Objective.KillBoss</t>
+  </si>
+  <si>
+    <t>Kill the Aberration</t>
+  </si>
+  <si>
+    <t>Mate a Aberração</t>
+  </si>
+  <si>
+    <t>Common.ReturnMedal</t>
+  </si>
+  <si>
+    <t>Return Medal</t>
+  </si>
+  <si>
+    <t>Medalha do Retorno</t>
   </si>
 </sst>
 </file>
@@ -865,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,333 +1249,451 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>75</v>
+      <c r="A28" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>78</v>
+      <c r="A31" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>81</v>
+      <c r="A34" s="1" t="s">
+        <v>150</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>118</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>83</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>119</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="A37" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>85</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>121</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>86</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>122</v>
-      </c>
+        <v>82</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>87</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="A40" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>88</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>125</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>90</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="A43" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C47" s="1" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B49" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>140</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>151</v>
+        <v>174</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>160</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B58" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>163</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="B61" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>164</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>165</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>166</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>167</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>168</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>169</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>170</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>171</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>173</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Two player. Fixed Camera. Tested everything. IT WORKS.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="206">
   <si>
     <t>Default</t>
   </si>
@@ -586,6 +586,57 @@
   </si>
   <si>
     <t>Medalha do Retorno</t>
+  </si>
+  <si>
+    <t>Learn how to use the fireball!</t>
+  </si>
+  <si>
+    <t>Aprenda a usar a Bola de Fogo!</t>
+  </si>
+  <si>
+    <t>Get the fireball spell, and use it to explore the abandoned ruins in the forest.</t>
+  </si>
+  <si>
+    <t>Obtenha a magia da bola de fogo e use-a para explorar as ruínas na floresta.</t>
+  </si>
+  <si>
+    <t>You learned how to use the fireball!</t>
+  </si>
+  <si>
+    <t>Você aprendeu a usar a bola de fogo!</t>
+  </si>
+  <si>
+    <t>Get the Boomerang</t>
+  </si>
+  <si>
+    <t>Get the boomerang on the dark forest, and learn how to control it to defeat enemies.</t>
+  </si>
+  <si>
+    <t>Obtenha o bumerangue na floresta negra, e aprenda a controlá-lo para destruir inimigos.</t>
+  </si>
+  <si>
+    <t>You got the boomerang!</t>
+  </si>
+  <si>
+    <t>Você obteve o bumerangue!</t>
+  </si>
+  <si>
+    <t>Kill the boss</t>
+  </si>
+  <si>
+    <t>Mate o chefe</t>
+  </si>
+  <si>
+    <t>Use all your weapons and knowledge to kill the boss.</t>
+  </si>
+  <si>
+    <t>Use suas armas e conhecimento para matar o chefe.</t>
+  </si>
+  <si>
+    <t>Boss killed!</t>
+  </si>
+  <si>
+    <t>Chefe morto!</t>
   </si>
 </sst>
 </file>
@@ -939,8 +990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,64 +1380,100 @@
       <c r="A35" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="B37" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>82</v>
       </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>83</v>
       </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="B41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>84</v>
       </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="B42" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="B43" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">

</xml_diff>

<commit_message>
Fixed objectives on every mission.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="209">
   <si>
     <t>Default</t>
   </si>
@@ -637,6 +637,15 @@
   </si>
   <si>
     <t>Chefe morto!</t>
+  </si>
+  <si>
+    <t>Objective.LightTorches</t>
+  </si>
+  <si>
+    <t>Light up torches</t>
+  </si>
+  <si>
+    <t>Acenda as tochas</t>
   </si>
 </sst>
 </file>
@@ -988,10 +997,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1783,6 +1792,20 @@
         <v>118</v>
       </c>
     </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>206</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed worm animations with texture! Also added dialog to chests.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="224">
   <si>
     <t>Default</t>
   </si>
@@ -646,6 +646,51 @@
   </si>
   <si>
     <t>Acenda as tochas</t>
+  </si>
+  <si>
+    <t>ItemGet.Sword</t>
+  </si>
+  <si>
+    <t>ItemGet.Boomerang</t>
+  </si>
+  <si>
+    <t>ItemGet.Bow</t>
+  </si>
+  <si>
+    <t>ItemGet.Fireball</t>
+  </si>
+  <si>
+    <t>ItemGet.Already</t>
+  </si>
+  <si>
+    <t>You got the sword!</t>
+  </si>
+  <si>
+    <t>You got the bow!</t>
+  </si>
+  <si>
+    <t>Você obteve a espada!</t>
+  </si>
+  <si>
+    <t>You got the fireball spell!</t>
+  </si>
+  <si>
+    <t>Você obteve a magia bola de fogo!</t>
+  </si>
+  <si>
+    <t>Você já tinha esta arma!</t>
+  </si>
+  <si>
+    <t>You already had this weapon!</t>
+  </si>
+  <si>
+    <t>ItemGet.Unknown</t>
+  </si>
+  <si>
+    <t>You got an unknown item!</t>
+  </si>
+  <si>
+    <t>Você obteve um item desconhecido!</t>
   </si>
 </sst>
 </file>
@@ -997,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,7 +1849,70 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C73" s="2"/>
+      <c r="A73" t="s">
+        <v>209</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>210</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>211</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>212</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>213</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>221</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>223</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Fixed objective menu alignment.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Postgrad\Projeto Final\Project\quest-for-the-crown-3d\Game\Assets\Localization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="239">
   <si>
     <t>Default</t>
   </si>
@@ -82,9 +87,6 @@
     <t>This is a test dialog.</t>
   </si>
   <si>
-    <t>New Game</t>
-  </si>
-  <si>
     <t>Load Game</t>
   </si>
   <si>
@@ -133,9 +135,6 @@
     <t>Este é outro diálogo teste.</t>
   </si>
   <si>
-    <t>Novo Jogo</t>
-  </si>
-  <si>
     <t>Carregar Jogo</t>
   </si>
   <si>
@@ -695,6 +694,48 @@
   </si>
   <si>
     <t>Objetivos</t>
+  </si>
+  <si>
+    <t>Dois Jogadores</t>
+  </si>
+  <si>
+    <t>Two Players</t>
+  </si>
+  <si>
+    <t>Menu.TwoPlayers</t>
+  </si>
+  <si>
+    <t>Menu.OnePlayer</t>
+  </si>
+  <si>
+    <t>One Player</t>
+  </si>
+  <si>
+    <t>Um Jogador</t>
+  </si>
+  <si>
+    <t>Menu.Back</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Voltar</t>
+  </si>
+  <si>
+    <t>Menu.About</t>
+  </si>
+  <si>
+    <t>Credits</t>
+  </si>
+  <si>
+    <t>Créditos</t>
+  </si>
+  <si>
+    <t>Start Game</t>
+  </si>
+  <si>
+    <t>Começar Jogo</t>
   </si>
 </sst>
 </file>
@@ -802,7 +843,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -837,7 +878,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1046,10 +1087,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,7 +1119,7 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1089,7 +1130,7 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1097,10 +1138,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>237</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1108,10 +1149,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1119,10 +1160,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1130,10 +1171,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1141,10 +1182,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1152,10 +1193,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1163,10 +1204,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1174,10 +1215,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1185,10 +1226,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1196,10 +1237,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1207,10 +1248,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,10 +1259,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1229,10 +1270,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1240,10 +1281,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1251,10 +1292,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1262,672 +1303,719 @@
         <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="D22" s="2"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>186</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>123</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>204</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="C72" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>214</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>219</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="B78" s="1" t="s">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="B79" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="C79" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B79" s="1" t="s">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>226</v>
-      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Added some flavor to the mission descriptions.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Postgrad\Projeto Final\Project\quest-for-the-crown-3d\Game\Assets\Localization\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -273,15 +268,6 @@
     <t>Kill Some Worms</t>
   </si>
   <si>
-    <t>Worms Attacked the Forest. Kill them.</t>
-  </si>
-  <si>
-    <t>Get your bow!</t>
-  </si>
-  <si>
-    <t>Get your bow and kill a few long ranged enemies.</t>
-  </si>
-  <si>
     <t>Bow Practice</t>
   </si>
   <si>
@@ -321,15 +307,6 @@
     <t>Mate algumas Minhocas</t>
   </si>
   <si>
-    <t>Minhocas atacaram a floresta. Mate-as.</t>
-  </si>
-  <si>
-    <t>Obtenha seu arco!</t>
-  </si>
-  <si>
-    <t>Obtenha seu arco e mate alguns inimigos com ataques de longo alcance.</t>
-  </si>
-  <si>
     <t>Prática de Arco e Flecha</t>
   </si>
   <si>
@@ -468,15 +445,6 @@
     <t>Mission.Complete02</t>
   </si>
   <si>
-    <t>You killed 15 worms!</t>
-  </si>
-  <si>
-    <t>Você matou 15 Minhocas!</t>
-  </si>
-  <si>
-    <t>You got your bow!</t>
-  </si>
-  <si>
     <t>Você obteve o arco!</t>
   </si>
   <si>
@@ -588,12 +556,6 @@
     <t>Aprenda a usar a Bola de Fogo!</t>
   </si>
   <si>
-    <t>Get the fireball spell, and use it to explore the abandoned ruins in the forest.</t>
-  </si>
-  <si>
-    <t>Obtenha a magia da bola de fogo e use-a para explorar as ruínas na floresta.</t>
-  </si>
-  <si>
     <t>You learned how to use the fireball!</t>
   </si>
   <si>
@@ -603,36 +565,12 @@
     <t>Get the Boomerang</t>
   </si>
   <si>
-    <t>Get the boomerang on the dark forest, and learn how to control it to defeat enemies.</t>
-  </si>
-  <si>
-    <t>Obtenha o bumerangue na floresta negra, e aprenda a controlá-lo para destruir inimigos.</t>
-  </si>
-  <si>
     <t>You got the boomerang!</t>
   </si>
   <si>
     <t>Você obteve o bumerangue!</t>
   </si>
   <si>
-    <t>Kill the boss</t>
-  </si>
-  <si>
-    <t>Mate o chefe</t>
-  </si>
-  <si>
-    <t>Use all your weapons and knowledge to kill the boss.</t>
-  </si>
-  <si>
-    <t>Use suas armas e conhecimento para matar o chefe.</t>
-  </si>
-  <si>
-    <t>Boss killed!</t>
-  </si>
-  <si>
-    <t>Chefe morto!</t>
-  </si>
-  <si>
     <t>Objective.LightTorches</t>
   </si>
   <si>
@@ -736,6 +674,63 @@
   </si>
   <si>
     <t>Começar Jogo</t>
+  </si>
+  <si>
+    <t>Giant Worms Attacked the Forest to the north of the kingdom. People are worried, since the worms never were so agressive. Some say the cause may be magical, maybe it's the crown?</t>
+  </si>
+  <si>
+    <t>Minhocas Gigantes invadiram a floresta ao norte do reino. Algumas pessoas estão preocupadas, pois as minhocas nunca foram tão agressivas. Alguns dizem que a causa pode ser mágica, quem sabe seja a coroa?</t>
+  </si>
+  <si>
+    <t>You controlled the Giant Worm population!</t>
+  </si>
+  <si>
+    <t>Você controlou a população de minhocas agressivas!</t>
+  </si>
+  <si>
+    <t>Get a bow!</t>
+  </si>
+  <si>
+    <t>Obtenha um arco!</t>
+  </si>
+  <si>
+    <t>Some villagers tell a legend, that to the east of the forest there is a bow that doesn't need arrows - it creates arrows using magic! Investigate it, but beware, since magic creatures roam the area.</t>
+  </si>
+  <si>
+    <t>Alguns aldeões lhe contam uma lenda, que diz que ao leste da floresta está um arco que não necessita de flechas - ele cria flechas usando magía! Investigue, mas tenha cuidado, pois criatoras mágicas habitam esta área.</t>
+  </si>
+  <si>
+    <t>You got the magic bow!</t>
+  </si>
+  <si>
+    <t>Você obteve o arco mágico!</t>
+  </si>
+  <si>
+    <t>Deep in the forest you found some forgotten ruins. The inscriptions on the entrance say "Learn the Spell here inside, and light the path to the truth". Maybe the ruins hold a clue on how to find the crown?</t>
+  </si>
+  <si>
+    <t>Nas profundezas da floresta, você acha algumas ruínas esquecidas. As inscrições na entrada dizem: "Aprenda a Magia que aqui está, e ilumine o caminho para a verdade". Quem sabe as ruínas guardam alguma pista para achar a coroa?</t>
+  </si>
+  <si>
+    <t>Deep in the dark forest, lies a possessed boomerang, that can be controled with magic. Add it to your arsenal, and investigate the deep forest.</t>
+  </si>
+  <si>
+    <t>Nas profundezas da floresta, está um bumerangue possuido, que pode ser controlado com mágica. Adicione-o ao seu arsenal, e investigue a floresta escura.</t>
+  </si>
+  <si>
+    <t>Kill the aberration</t>
+  </si>
+  <si>
+    <t>On the ruins, you found a secret passage to the deepest part of the forest. There lives a grotesque creature, that is probably the cause of all the troubles on the forest. Get rid of it, and save the forest.</t>
+  </si>
+  <si>
+    <t>Nas ruínas, você acha uma passagem secreta para a parte mais profunda da floresta. Ali vive uma criatura grotesca, que possivelmente é a causa de todos os problemas na floresta. Livre-se dela e salve a floresta.</t>
+  </si>
+  <si>
+    <t>Aberration Killed!</t>
+  </si>
+  <si>
+    <t>Aberração Morta!</t>
   </si>
 </sst>
 </file>
@@ -843,7 +838,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -878,7 +873,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1089,8 +1084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1138,10 +1133,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="C4" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1400,13 +1395,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1417,7 +1412,7 @@
         <v>83</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1425,21 +1420,21 @@
         <v>74</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>84</v>
+        <v>220</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>100</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>149</v>
+        <v>222</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>150</v>
+        <v>223</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1447,10 +1442,10 @@
         <v>75</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>85</v>
+        <v>224</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>101</v>
+        <v>225</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1458,21 +1453,21 @@
         <v>76</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>86</v>
+        <v>226</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>102</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>151</v>
+        <v>228</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>152</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1480,10 +1475,10 @@
         <v>79</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1491,21 +1486,21 @@
         <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>189</v>
+        <v>230</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>190</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1513,10 +1508,10 @@
         <v>77</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1524,21 +1519,21 @@
         <v>78</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>194</v>
+        <v>232</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>195</v>
+        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1546,10 +1541,10 @@
         <v>81</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1557,461 +1552,461 @@
         <v>82</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>200</v>
+        <v>235</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>202</v>
+        <v>237</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>203</v>
+        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>208</v>
+        <v>189</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>209</v>
+        <v>190</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>210</v>
+        <v>191</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>192</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>218</v>
+        <v>199</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>220</v>
+        <v>201</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>221</v>
+        <v>202</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>222</v>
+        <v>203</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>223</v>
+        <v>204</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>226</v>
+        <v>207</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>225</v>
+        <v>206</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>228</v>
+        <v>209</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>229</v>
+        <v>210</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>231</v>
+        <v>212</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>232</v>
+        <v>213</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Small visual adjustments and tips.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="242">
   <si>
     <t>Default</t>
   </si>
@@ -731,6 +731,15 @@
   </si>
   <si>
     <t>Aberração Morta!</t>
+  </si>
+  <si>
+    <t>UI.OpenMissionSelection</t>
+  </si>
+  <si>
+    <t>Press the [ACTION] button to open the Mission Selection.</t>
+  </si>
+  <si>
+    <t>Pressione o botão [AÇÃO] para abrir a Seleção de Missões.</t>
   </si>
 </sst>
 </file>
@@ -1084,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2009,6 +2018,17 @@
         <v>217</v>
       </c>
     </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
     </row>

</xml_diff>

<commit_message>
Torch bugfixes, text fixes, Magypus sound fix.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Postgrad\Projeto Final\Project\quest-for-the-crown-3d\Game\Assets\Localization\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -697,9 +702,6 @@
     <t>Some villagers tell a legend, that to the east of the forest there is a bow that doesn't need arrows - it creates arrows using magic! Investigate it, but beware, since magic creatures roam the area.</t>
   </si>
   <si>
-    <t>Alguns aldeões lhe contam uma lenda, que diz que ao leste da floresta está um arco que não necessita de flechas - ele cria flechas usando magía! Investigue, mas tenha cuidado, pois criatoras mágicas habitam esta área.</t>
-  </si>
-  <si>
     <t>You got the magic bow!</t>
   </si>
   <si>
@@ -740,6 +742,9 @@
   </si>
   <si>
     <t>Pressione o botão [AÇÃO] para abrir a Seleção de Missões.</t>
+  </si>
+  <si>
+    <t>Alguns aldeões lhe contam uma lenda, que diz que ao leste da floresta está um arco que não necessita de flechas - ele cria flechas usando magia! Investigue, mas tenha cuidado, pois criatoras mágicas habitam esta área.</t>
   </si>
 </sst>
 </file>
@@ -847,7 +852,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -882,7 +887,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1093,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,7 +1470,7 @@
         <v>226</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>227</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1473,10 +1478,10 @@
         <v>142</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1495,10 +1500,10 @@
         <v>80</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1528,10 +1533,10 @@
         <v>78</v>
       </c>
       <c r="B39" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,7 +1555,7 @@
         <v>81</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>174</v>
@@ -1561,10 +1566,10 @@
         <v>82</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>235</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1572,10 +1577,10 @@
         <v>148</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2020,13 +2025,13 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="B84" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="B84" s="1" t="s">
+      <c r="C84" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Continue Mission and Quit to Camp buttons on UI.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="246">
   <si>
     <t>Default</t>
   </si>
@@ -745,6 +745,18 @@
   </si>
   <si>
     <t>Alguns aldeões lhe contam uma lenda, que diz que ao leste da floresta está um arco que não necessita de flechas - ele cria flechas usando magia! Investigue, mas tenha cuidado, pois criatoras mágicas habitam esta área.</t>
+  </si>
+  <si>
+    <t>Option.BackToGame</t>
+  </si>
+  <si>
+    <t>Continue Mission</t>
+  </si>
+  <si>
+    <t>Continuar Missão</t>
+  </si>
+  <si>
+    <t>Option.BackToCamp</t>
   </si>
 </sst>
 </file>
@@ -1098,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,6 +2046,31 @@
         <v>240</v>
       </c>
     </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B87" s="1"/>
+    </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
     </row>

</xml_diff>

<commit_message>
Exit button on title screen.
</commit_message>
<xml_diff>
--- a/Game/Assets/Localization/LanguageData.xlsx
+++ b/Game/Assets/Localization/LanguageData.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Postgrad\Projeto Final\Project\quest-for-the-crown-3d\Game\Assets\Localization\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="249">
   <si>
     <t>Default</t>
   </si>
@@ -757,6 +752,15 @@
   </si>
   <si>
     <t>Option.BackToCamp</t>
+  </si>
+  <si>
+    <t>Menu.Exit</t>
+  </si>
+  <si>
+    <t>Quit Game</t>
+  </si>
+  <si>
+    <t>Sair do Jogo</t>
   </si>
 </sst>
 </file>
@@ -864,7 +868,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -899,7 +903,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1111,7 +1115,7 @@
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2069,7 +2073,15 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="1"/>
+      <c r="A87" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>

</xml_diff>